<commit_message>
Add representing year for AMI schema
</commit_message>
<xml_diff>
--- a/android-project-db-schema.xlsx
+++ b/android-project-db-schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vmorskyi/GitProjects/android-genymotion-backend/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0291265C-9839-F84A-A3F9-BD299C458984}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71CDD65C-E598-2346-8AA1-7CD83E60701A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="980" windowWidth="40920" windowHeight="25500" xr2:uid="{933F3ADF-53C7-3646-973D-CD8F011F3627}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>PK</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>Game UUID</t>
+  </si>
+  <si>
+    <t>AMI</t>
+  </si>
+  <si>
+    <t>Amazon Machine Image</t>
+  </si>
+  <si>
+    <t>AMI ID</t>
   </si>
 </sst>
 </file>
@@ -313,8 +322,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F0145DC-E91F-F748-A70B-3DEA5108C4BC}" name="Table1" displayName="Table1" ref="A1:G4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
-  <autoFilter ref="A1:G4" xr:uid="{7F0145DC-E91F-F748-A70B-3DEA5108C4BC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7F0145DC-E91F-F748-A70B-3DEA5108C4BC}" name="Table1" displayName="Table1" ref="A1:G5" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A1:G5" xr:uid="{7F0145DC-E91F-F748-A70B-3DEA5108C4BC}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{761658EA-DDF0-6043-85B7-CFA5974AA6BB}" name="Entity" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{3954F9C8-F2B6-204B-9B79-080DF1695339}" name="PK" dataDxfId="7"/>
@@ -645,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3EEBE2BF-957A-9F48-BF28-7DCE567F1B22}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.5" defaultRowHeight="27" x14ac:dyDescent="0.35"/>
@@ -713,10 +722,10 @@
         <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -746,6 +755,17 @@
       </c>
       <c r="G4" s="1" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>